<commit_message>
Added Franc to the list of participants
</commit_message>
<xml_diff>
--- a/paying participants updated.xlsx
+++ b/paying participants updated.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>Nb</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Kamga Jaures</t>
+  </si>
+  <si>
+    <t>Nsini Franc</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +537,7 @@
         <v>200</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H23" si="0">E3-G3-300</f>
+        <f t="shared" ref="H3:H25" si="0">E3-G3-300</f>
         <v>0</v>
       </c>
     </row>
@@ -1070,6 +1076,60 @@
       <c r="H23">
         <f t="shared" si="0"/>
         <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>691348635</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <v>500</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>658253270</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <v>500</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unique_together constraint from tournamentplayer model
</commit_message>
<xml_diff>
--- a/paying participants updated.xlsx
+++ b/paying participants updated.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Nb</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Mabou Fotso Kevin</t>
   </si>
   <si>
-    <t>Rikam Yvanol</t>
-  </si>
-  <si>
     <t>Mbame Mbame Martin</t>
   </si>
   <si>
@@ -127,6 +124,15 @@
   </si>
   <si>
     <t>Nsini Franc</t>
+  </si>
+  <si>
+    <t>Nguemo Aymard</t>
+  </si>
+  <si>
+    <t>Miendjem Thierry</t>
+  </si>
+  <si>
+    <t>Rikam Giovanni</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -498,7 +504,7 @@
         <v>694494629</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>500</v>
@@ -525,7 +531,7 @@
         <v>699003156</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>500</v>
@@ -537,7 +543,7 @@
         <v>200</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H25" si="0">E3-G3-300</f>
+        <f t="shared" ref="H3:H27" si="0">E3-G3-300</f>
         <v>0</v>
       </c>
     </row>
@@ -552,7 +558,7 @@
         <v>657407989</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>500</v>
@@ -579,7 +585,7 @@
         <v>693851447</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>350</v>
@@ -606,7 +612,7 @@
         <v>694865719</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>300</v>
@@ -633,7 +639,7 @@
         <v>658312450</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>500</v>
@@ -660,7 +666,7 @@
         <v>657489972</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <v>350</v>
@@ -687,7 +693,7 @@
         <v>675366970</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>500</v>
@@ -714,7 +720,7 @@
         <v>657936031</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <v>500</v>
@@ -735,13 +741,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>655372422</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <v>300</v>
@@ -762,13 +768,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>697720509</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <v>300</v>
@@ -789,13 +795,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>674743317</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13">
         <v>300</v>
@@ -816,13 +822,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>650469243</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14">
         <v>1000</v>
@@ -843,13 +849,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>692201677</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>300</v>
@@ -870,13 +876,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>695044180</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>1000</v>
@@ -897,13 +903,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>690839895</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17">
         <v>300</v>
@@ -924,13 +930,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>694993298</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18">
         <v>300</v>
@@ -951,13 +957,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>691674935</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19">
         <v>500</v>
@@ -978,13 +984,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>691569975</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <v>500</v>
@@ -1005,10 +1011,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <v>500</v>
@@ -1029,13 +1035,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>698207148</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>350</v>
@@ -1056,13 +1062,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>696374091</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23">
         <v>350</v>
@@ -1083,13 +1089,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>691348635</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <v>500</v>
@@ -1110,13 +1116,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <v>658253270</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25">
         <v>500</v>
@@ -1130,6 +1136,60 @@
       <c r="H25">
         <f t="shared" si="0"/>
         <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>699027926</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26">
+        <v>300</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>658528672</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <v>300</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>